<commit_message>
aSQA updated with text
</commit_message>
<xml_diff>
--- a/SAiP/Module2/H5CloudArchitectualEvaluation/part2/aSQA.xlsx
+++ b/SAiP/Module2/H5CloudArchitectualEvaluation/part2/aSQA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
   <si>
     <t>Avalibility</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Security</t>
+  </si>
+  <si>
+    <t>Change Log:</t>
+  </si>
+  <si>
+    <t>Startup of project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security pacakage -&gt; User authentication added. </t>
   </si>
 </sst>
 </file>
@@ -131,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -148,6 +157,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T24"/>
+  <dimension ref="B2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,6 +910,51 @@
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
     </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+    </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
@@ -1320,11 +1377,58 @@
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
     </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="J16:N16"/>
     <mergeCell ref="P16:T16"/>
+    <mergeCell ref="C12:T13"/>
+    <mergeCell ref="C25:T26"/>
     <mergeCell ref="J3:N3"/>
     <mergeCell ref="P3:T3"/>
     <mergeCell ref="D3:H3"/>

</xml_diff>

<commit_message>
aSQA updated with H3
</commit_message>
<xml_diff>
--- a/SAiP/Module2/H5CloudArchitectualEvaluation/part2/aSQA.xlsx
+++ b/SAiP/Module2/H5CloudArchitectualEvaluation/part2/aSQA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="21">
   <si>
     <t>Avalibility</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve">Security pacakage -&gt; User authentication added. </t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>Avalibility spike -&gt; Possibilities to improve Avalibility explored.</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T26"/>
+  <dimension ref="A2:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +989,7 @@
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
     </row>
-    <row r="17" spans="2:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="2" t="s">
@@ -1032,7 +1038,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>1</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>2</v>
       </c>
@@ -1203,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
@@ -1317,7 +1323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
@@ -1374,10 +1380,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>16</v>
       </c>
@@ -1402,7 +1408,7 @@
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1422,18 +1428,529 @@
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
     </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="J30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="P30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O31" s="3"/>
+      <c r="P31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U31" s="3"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
+      <c r="F32" s="1">
+        <f xml:space="preserve">  5 - MAX(0, (D32-E32))</f>
+        <v>2</v>
+      </c>
+      <c r="G32" s="1">
+        <v>5</v>
+      </c>
+      <c r="H32" s="1">
+        <f xml:space="preserve"> ROUND(  ((6-F32) * (G32/5)),0 )</f>
+        <v>4</v>
+      </c>
+      <c r="J32" s="1">
+        <v>5</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1</v>
+      </c>
+      <c r="L32" s="1">
+        <f xml:space="preserve">  5 - MAX(0, (J32-K32))</f>
+        <v>1</v>
+      </c>
+      <c r="M32" s="1">
+        <v>5</v>
+      </c>
+      <c r="N32" s="1">
+        <f xml:space="preserve"> ROUND(  ((6-L32) * (M32/5)),0 )</f>
+        <v>5</v>
+      </c>
+      <c r="P32" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+      <c r="R32" s="1">
+        <f xml:space="preserve">  5 - MAX(0, (P32-Q32))</f>
+        <v>3</v>
+      </c>
+      <c r="S32" s="1">
+        <v>3</v>
+      </c>
+      <c r="T32" s="1">
+        <f xml:space="preserve"> ROUND(  ((6-R32) * (S32/5)),0 )</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" ref="F33:F37" si="12" xml:space="preserve">  5 - MAX(0, (D33-E33))</f>
+        <v>4</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" ref="H33:H37" si="13" xml:space="preserve"> ROUND(  ((6-F33) * (G33/5)),0 )</f>
+        <v>2</v>
+      </c>
+      <c r="J33" s="1">
+        <v>5</v>
+      </c>
+      <c r="K33" s="1">
+        <v>2</v>
+      </c>
+      <c r="L33" s="1">
+        <f t="shared" ref="L33:L37" si="14" xml:space="preserve">  5 - MAX(0, (J33-K33))</f>
+        <v>2</v>
+      </c>
+      <c r="M33" s="1">
+        <v>5</v>
+      </c>
+      <c r="N33" s="1">
+        <f t="shared" ref="N33:N37" si="15" xml:space="preserve"> ROUND(  ((6-L33) * (M33/5)),0 )</f>
+        <v>4</v>
+      </c>
+      <c r="P33" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>1</v>
+      </c>
+      <c r="R33" s="1">
+        <f t="shared" ref="R33:R37" si="16" xml:space="preserve">  5 - MAX(0, (P33-Q33))</f>
+        <v>3</v>
+      </c>
+      <c r="S33" s="1">
+        <v>3</v>
+      </c>
+      <c r="T33" s="1">
+        <f t="shared" ref="T33:T37" si="17" xml:space="preserve"> ROUND(  ((6-R33) * (S33/5)),0 )</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="1">
+        <v>4</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="G34" s="1">
+        <v>4</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1</v>
+      </c>
+      <c r="L34" s="1">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="M34" s="1">
+        <v>3</v>
+      </c>
+      <c r="N34" s="1">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="P34" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>1</v>
+      </c>
+      <c r="R34" s="1">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="S34" s="1">
+        <v>3</v>
+      </c>
+      <c r="T34" s="1">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="1">
+        <v>4</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="G35" s="1">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="J35" s="1">
+        <v>2</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1</v>
+      </c>
+      <c r="L35" s="1">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="M35" s="1">
+        <v>1</v>
+      </c>
+      <c r="N35" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>1</v>
+      </c>
+      <c r="R35" s="1">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="S35" s="1">
+        <v>3</v>
+      </c>
+      <c r="T35" s="1">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="1">
+        <v>5</v>
+      </c>
+      <c r="E36" s="1">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>5</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="J36" s="1">
+        <v>3</v>
+      </c>
+      <c r="K36" s="1">
+        <v>1</v>
+      </c>
+      <c r="L36" s="1">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="M36" s="1">
+        <v>3</v>
+      </c>
+      <c r="N36" s="1">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="P36" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>1</v>
+      </c>
+      <c r="R36" s="1">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="S36" s="1">
+        <v>5</v>
+      </c>
+      <c r="T36" s="1">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="G37" s="1">
+        <v>3</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="J37" s="1">
+        <v>2</v>
+      </c>
+      <c r="K37" s="1">
+        <v>2</v>
+      </c>
+      <c r="L37" s="1">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1</v>
+      </c>
+      <c r="N37" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="P37" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>1</v>
+      </c>
+      <c r="R37" s="1">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="S37" s="1">
+        <v>5</v>
+      </c>
+      <c r="T37" s="1">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="C39:T40"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="J16:N16"/>
     <mergeCell ref="P16:T16"/>
     <mergeCell ref="C12:T13"/>
     <mergeCell ref="C25:T26"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="P30:T30"/>
     <mergeCell ref="J3:N3"/>
     <mergeCell ref="P3:T3"/>
     <mergeCell ref="D3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H10">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:N10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T5:T10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:H23">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1445,7 +1962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5:N10">
+  <conditionalFormatting sqref="N18:N23">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1457,7 +1974,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T5:T10">
+  <conditionalFormatting sqref="T18:T23">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1469,7 +1986,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18:H23">
+  <conditionalFormatting sqref="H32:H37">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1481,7 +1998,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18:N23">
+  <conditionalFormatting sqref="N32:N37">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1493,7 +2010,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T18:T23">
+  <conditionalFormatting sqref="T32:T37">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>